<commit_message>
add ifop and elabe polls (02/10-11)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Library/CloudStorage/Dropbox/PollsFrance2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E362B6F-D56E-A14D-B743-782DD29D5365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C56A981-9746-3146-9451-4B418A017EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35540" yWindow="2540" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -152,6 +152,15 @@
   </si>
   <si>
     <t>thierry breton</t>
+  </si>
+  <si>
+    <t>julien denormandie</t>
+  </si>
+  <si>
+    <t>clément beaune</t>
+  </si>
+  <si>
+    <t>valérie hayer</t>
   </si>
 </sst>
 </file>
@@ -520,9 +529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
   <dimension ref="A1:AG467"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
+      <selection pane="bottomLeft" activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1462,7 +1471,7 @@
         <v>800</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="2">
         <v>1</v>
@@ -1536,7 +1545,7 @@
         <v>834</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="2">
         <v>1</v>
@@ -1610,7 +1619,7 @@
         <v>1209</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="2">
         <v>1</v>
@@ -1653,72 +1662,361 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="12:33" x14ac:dyDescent="0.2">
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="12:33" x14ac:dyDescent="0.2">
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="12:33" x14ac:dyDescent="0.2">
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="12:33" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>2024</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16">
+        <v>900</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>7.5</v>
+      </c>
+      <c r="P16">
+        <v>3</v>
+      </c>
+      <c r="Q16">
+        <v>8.5</v>
+      </c>
+      <c r="R16">
+        <v>10.5</v>
+      </c>
+      <c r="S16">
+        <v>19</v>
+      </c>
+      <c r="T16">
+        <v>7.5</v>
+      </c>
+      <c r="U16">
+        <v>1.5</v>
+      </c>
+      <c r="V16">
+        <v>28.5</v>
+      </c>
+      <c r="W16">
+        <v>6</v>
+      </c>
+      <c r="X16">
+        <v>7</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>2024</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17">
+        <v>900</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N17">
+        <v>1.5</v>
+      </c>
+      <c r="O17">
+        <v>7</v>
+      </c>
+      <c r="P17">
+        <v>3.5</v>
+      </c>
+      <c r="Q17">
+        <v>8</v>
+      </c>
+      <c r="R17">
+        <v>9.5</v>
+      </c>
+      <c r="S17">
+        <v>19</v>
+      </c>
+      <c r="T17">
+        <v>7</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>29</v>
+      </c>
+      <c r="W17">
+        <v>6.5</v>
+      </c>
+      <c r="X17">
+        <v>8</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>2024</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18">
+        <v>900</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>8</v>
+      </c>
+      <c r="P18">
+        <v>3.5</v>
+      </c>
+      <c r="Q18">
+        <v>8</v>
+      </c>
+      <c r="R18">
+        <v>10.5</v>
+      </c>
+      <c r="S18">
+        <v>18</v>
+      </c>
+      <c r="T18">
+        <v>7.5</v>
+      </c>
+      <c r="U18">
+        <v>1.5</v>
+      </c>
+      <c r="V18">
+        <v>28</v>
+      </c>
+      <c r="W18">
+        <v>6</v>
+      </c>
+      <c r="X18">
+        <v>8</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>2024</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19">
+        <v>800</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N19">
+        <v>1.5</v>
+      </c>
+      <c r="O19">
+        <v>9</v>
+      </c>
+      <c r="P19">
+        <v>2.5</v>
+      </c>
+      <c r="Q19">
+        <v>9.5</v>
+      </c>
+      <c r="R19">
+        <v>9</v>
+      </c>
+      <c r="S19">
+        <v>16.5</v>
+      </c>
+      <c r="T19">
+        <v>8</v>
+      </c>
+      <c r="U19">
+        <v>3</v>
+      </c>
+      <c r="V19">
+        <v>27.5</v>
+      </c>
+      <c r="W19">
+        <v>5</v>
+      </c>
+      <c r="X19">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="U20" s="1"/>
       <c r="AG20" s="1"/>
     </row>
-    <row r="21" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="12:33" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>

</xml_diff>

<commit_message>
update with yougov poll (2/7); update temporary n
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Library/CloudStorage/Dropbox/PollsFrance2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C56A981-9746-3146-9451-4B418A017EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71414D50-55E4-284C-8C04-B276617B069C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35540" yWindow="2540" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>year</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>valérie hayer</t>
+  </si>
+  <si>
+    <t>yougov</t>
   </si>
 </sst>
 </file>
@@ -529,9 +532,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
   <dimension ref="A1:AG467"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="V22" sqref="V22"/>
+      <selection pane="bottomLeft" activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1690,10 +1693,10 @@
         <v>21</v>
       </c>
       <c r="J16">
-        <v>900</v>
+        <v>576</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="2">
         <v>1</v>
@@ -1738,7 +1741,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1767,10 +1770,10 @@
         <v>21</v>
       </c>
       <c r="J17">
-        <v>900</v>
+        <v>582</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="2">
         <v>1</v>
@@ -1815,7 +1818,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>13</v>
       </c>
@@ -1844,10 +1847,10 @@
         <v>21</v>
       </c>
       <c r="J18">
-        <v>900</v>
+        <v>581</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="2">
         <v>1</v>
@@ -1892,7 +1895,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>14</v>
       </c>
@@ -1966,57 +1969,125 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="U20" s="1"/>
-      <c r="AG20" s="1"/>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>2024</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>29</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>7</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20">
+        <v>549</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>8</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>8</v>
+      </c>
+      <c r="R20">
+        <v>8</v>
+      </c>
+      <c r="S20">
+        <v>19</v>
+      </c>
+      <c r="T20">
+        <v>6</v>
+      </c>
+      <c r="U20">
+        <v>2</v>
+      </c>
+      <c r="V20">
+        <v>32</v>
+      </c>
+      <c r="W20">
+        <v>8</v>
+      </c>
+      <c r="X20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>

</xml_diff>